<commit_message>
Rename master branch venturecafe
</commit_message>
<xml_diff>
--- a/hw/BeerBeer_master_BOM_17feb13.xlsx
+++ b/hw/BeerBeer_master_BOM_17feb13.xlsx
@@ -347,7 +347,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -419,8 +419,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -432,7 +432,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -735,6 +735,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1472,7 +1475,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="46" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>